<commit_message>
update case study for two discount approaches
</commit_message>
<xml_diff>
--- a/survey/case study.xlsx
+++ b/survey/case study.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie Jones\Documents\GitHub\epfl-load-flexibility\survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/dev/load-flexibility/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{33B6EFC5-3749-47BE-9CC8-A898E22B909D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EF4FC6-0029-434F-ADAF-4A73C6B0A790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="384" yWindow="384" windowWidth="21600" windowHeight="11208"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="25740" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>hour</t>
   </si>
@@ -52,12 +53,18 @@
   <si>
     <t>Time difference</t>
   </si>
+  <si>
+    <t>discount relative to price at each time -- savings relative to desired time</t>
+  </si>
+  <si>
+    <t>discount relative to price at new time -- savings relative to standard price at new time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,13 +78,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,11 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,7 +155,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -343,43 +366,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>6.4</c:v>
+                  <c:v>11.347999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9679999999999982</c:v>
+                  <c:v>9.9159999999999968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.391999999999999</c:v>
+                  <c:v>7.3399999999999963</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47999999999999832</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.71999999999999886</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5919999999999987</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.1679999999999979</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.695999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.4159999999999995</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.5599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.3359999999999985</c:v>
+                  <c:v>5.4279999999999973</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -503,70 +499,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>-1.8240000000000016</c:v>
+                  <c:v>8.0719999999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3799999999999983</c:v>
+                  <c:v>11.275999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6399999999999992</c:v>
+                  <c:v>12.536</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8739999999999992</c:v>
+                  <c:v>12.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8639999999999985</c:v>
+                  <c:v>13.759999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6319999999999988</c:v>
+                  <c:v>14.527999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2319999999999993</c:v>
+                  <c:v>15.127999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7359999999999989</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.7259999999999982</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7939999999999989</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.35999999999999871</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.53999999999999915</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.9439999999999991</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6259999999999983</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7719999999999985</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.3119999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.4199999999999995</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.2519999999999989</c:v>
+                  <c:v>15.632</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4059999999999988</c:v>
+                  <c:v>12.301999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,6 +532,717 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-D1E6-4BD0-BBA6-F371AA1BFD0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="415848528"/>
+        <c:axId val="2006986048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="415848528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time difference [hours]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2006986048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2006986048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Relative savings [€/MWh]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="415848528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>No incentive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$22:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$22:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89999999999999858</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2399999999999984</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7099999999999973</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6199999999999974</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.4199999999999982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7094-B141-A4DC-6D11B2C8FD47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>20% discount</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$18:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$18:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-3.0520000000000032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.2620000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9579999999999984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.347999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7094-B141-A4DC-6D11B2C8FD47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>40% discount</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$10:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$10:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>12.936000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5960000000000036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4960000000000022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1060000000000016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4560000000000031</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1760000000000019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1760000000000019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33600000000000207</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.8860000000000028</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7094-B141-A4DC-6D11B2C8FD47}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -946,7 +1614,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1487,6 +2711,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C429A29-6908-034A-BFCF-02112D4B4BD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1799,16 +3066,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1827,8 +3094,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -1836,402 +3106,304 @@
       <c r="B2" s="1">
         <v>22.03</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C20" si="0">$B$22-B2</f>
-        <v>2.7099999999999973</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A47" si="1">A2+1</f>
+        <f t="shared" ref="A3:A47" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>20.12</v>
       </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>4.6199999999999974</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>19.22</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>5.52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>19.04</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>5.6999999999999993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>19.32</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>5.4199999999999982</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>20.73</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>4.009999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>25.05</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>-0.31000000000000227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>28.71</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>-3.9700000000000024</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>27.78</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>-3.0400000000000027</v>
-      </c>
       <c r="D10">
-        <f t="shared" ref="D8:D20" si="2">D11-1</f>
+        <f t="shared" ref="D10:D20" si="1">D11-1</f>
         <v>-12</v>
       </c>
-      <c r="F10">
-        <f>C10*0.6</f>
-        <v>-1.8240000000000016</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:F17" si="2">$B$22-$B10*0.6</f>
+        <v>8.0719999999999992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>22.44</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>2.2999999999999972</v>
-      </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>-11</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>-11</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F31" si="3">C11*0.6</f>
-        <v>1.3799999999999983</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>11.275999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>20.34</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>4.3999999999999986</v>
-      </c>
       <c r="D12">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="2"/>
-        <v>-10</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>2.6399999999999992</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12.536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>19.95</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>4.7899999999999991</v>
-      </c>
       <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="2"/>
-        <v>-9</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>2.8739999999999992</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>18.3</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>6.4399999999999977</v>
-      </c>
       <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>-8</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>3.8639999999999985</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>13.759999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>17.02</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>7.7199999999999989</v>
-      </c>
       <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="F15" s="2">
         <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>4.6319999999999988</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14.527999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>16.02</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>8.7199999999999989</v>
-      </c>
       <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="F16" s="2">
         <f t="shared" si="2"/>
-        <v>-6</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>5.2319999999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15.127999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>15.18</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>9.5599999999999987</v>
-      </c>
       <c r="D17">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>-5</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>5.7359999999999989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15.632</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>16.739999999999998</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f>D19-1</f>
         <v>-4</v>
       </c>
-      <c r="E18">
-        <f>C18*0.8</f>
-        <v>6.4</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="2">
+        <f>$B$22-$B18*0.8</f>
+        <v>11.347999999999999</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>18.53</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>6.2099999999999973</v>
-      </c>
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="E19">
-        <f t="shared" ref="E19:E30" si="4">C19*0.8</f>
-        <v>4.9679999999999982</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>3.7259999999999982</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="2">
+        <f t="shared" ref="E19:E21" si="3">$B$22-$B19*0.8</f>
+        <v>9.9159999999999968</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>21.75</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>2.9899999999999984</v>
-      </c>
       <c r="D20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
-        <v>2.391999999999999</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="2">
         <f t="shared" si="3"/>
-        <v>1.7939999999999989</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>7.3399999999999963</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>24.14</v>
-      </c>
-      <c r="C21">
-        <f>$B$22-B21</f>
-        <v>0.59999999999999787</v>
       </c>
       <c r="D21">
         <f>D22-1</f>
         <v>-1</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="4"/>
-        <v>0.47999999999999832</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="2">
         <f t="shared" si="3"/>
-        <v>0.35999999999999871</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5.4279999999999973</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>24.74</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>23.84</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <f>$B$22-B23</f>
         <v>0.89999999999999858</v>
       </c>
@@ -2239,91 +3411,67 @@
         <f>D22+1</f>
         <v>1</v>
       </c>
-      <c r="E23">
-        <f>($B$22-B23)*0.8</f>
-        <v>0.71999999999999886</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>0.53999999999999915</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>22.99</v>
       </c>
-      <c r="C24">
-        <f t="shared" ref="C24:C47" si="5">$B$22-B24</f>
+      <c r="C24" s="2">
+        <f t="shared" ref="C24:C30" si="4">$B$22-B24</f>
         <v>1.75</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D47" si="6">D23+1</f>
+        <f t="shared" ref="D24:D34" si="5">D23+1</f>
         <v>2</v>
       </c>
-      <c r="E24">
-        <f t="shared" ref="E24:E30" si="7">($B$22-B24)*0.8</f>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25">
         <v>21.5</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>3.2399999999999984</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="5"/>
-        <v>3.2399999999999984</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="7"/>
-        <v>2.5919999999999987</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>1.9439999999999991</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>22.03</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
+        <f t="shared" si="4"/>
+        <v>2.7099999999999973</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="5"/>
-        <v>2.7099999999999973</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="7"/>
-        <v>2.1679999999999979</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>1.6259999999999983</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>A26+1</f>
         <v>26</v>
@@ -2331,340 +3479,915 @@
       <c r="B27" s="1">
         <v>20.12</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6199999999999974</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="5"/>
-        <v>4.6199999999999974</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="7"/>
-        <v>3.695999999999998</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>2.7719999999999985</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>19.22</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
+        <f t="shared" si="4"/>
+        <v>5.52</v>
+      </c>
+      <c r="D28">
         <f t="shared" si="5"/>
-        <v>5.52</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="7"/>
-        <v>4.4159999999999995</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>3.3119999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>19.04</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
+        <f t="shared" si="4"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="5"/>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="7"/>
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>3.4199999999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>19.32</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4199999999999982</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="5"/>
-        <v>5.4199999999999982</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="7"/>
-        <v>4.3359999999999985</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>3.2519999999999989</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>20.73</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <f t="shared" si="5"/>
-        <v>4.009999999999998</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
-        <v>2.4059999999999988</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F31" s="2">
+        <f>$B$22-$B31*0.6</f>
+        <v>12.301999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>25.05</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <f t="shared" si="5"/>
-        <v>-0.31000000000000227</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="6"/>
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>28.71</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <f t="shared" si="5"/>
-        <v>-3.9700000000000024</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>27.78</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <f t="shared" si="5"/>
-        <v>-3.0400000000000027</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="6"/>
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>22.44</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="5"/>
-        <v>2.2999999999999972</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>20.34</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="5"/>
-        <v>4.3999999999999986</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>19.95</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="5"/>
-        <v>4.7899999999999991</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>18.3</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="5"/>
-        <v>6.4399999999999977</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>17.02</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="5"/>
-        <v>7.7199999999999989</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>16.02</v>
       </c>
-      <c r="C40">
-        <f t="shared" si="5"/>
-        <v>8.7199999999999989</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>15.18</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="5"/>
-        <v>9.5599999999999987</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>16.739999999999998</v>
       </c>
-      <c r="C42">
+    </row>
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>18.53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>24.14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>24.74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>23.84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>22.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54949767-DC6D-7C41-94D0-EFE137C8DA03}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A47" si="0">A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>19.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>25.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>28.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>27.78</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:D20" si="1">D11-1</f>
+        <v>-12</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:F31" si="2">$B10-$B$22*0.6</f>
+        <v>12.936000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>22.44</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>-11</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5960000000000036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>20.34</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="2"/>
+        <v>5.4960000000000022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>19.95</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="2"/>
+        <v>5.1060000000000016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4560000000000031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>17.02</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1760000000000019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>16.02</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1760000000000019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15.18</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.33600000000000207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="D18">
+        <f>D19-1</f>
+        <v>-4</v>
+      </c>
+      <c r="E18" s="2">
+        <f>$B18-$B$22*0.8</f>
+        <v>-3.0520000000000032</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18.53</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" ref="E19:E21" si="3">$B19-$B$22*0.8</f>
+        <v>-1.2620000000000005</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>21.75</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="3"/>
+        <v>1.9579999999999984</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>24.14</v>
+      </c>
+      <c r="D21">
+        <f>D22-1</f>
+        <v>-1</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="3"/>
+        <v>4.347999999999999</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>24.74</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>23.84</v>
+      </c>
+      <c r="C23" s="2">
+        <f>$B$22-B23</f>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="D23">
+        <f>D22+1</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>22.99</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" ref="C24:C30" si="4">$B$22-B24</f>
+        <v>1.75</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D34" si="5">D23+1</f>
+        <v>2</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>21.5</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>3.2399999999999984</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>22.03</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="4"/>
+        <v>2.7099999999999973</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>20.12</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6199999999999974</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>19.22</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="4"/>
+        <v>5.52</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>19.04</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="4"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4199999999999982</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>20.73</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="2"/>
+        <v>5.8860000000000028</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>25.05</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>28.71</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>27.78</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>22.44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>20.34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>17.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>16.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>16.739999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>18.53</v>
       </c>
-      <c r="C43">
-        <f t="shared" si="5"/>
-        <v>6.2099999999999973</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>21.75</v>
       </c>
-      <c r="C44">
-        <f t="shared" si="5"/>
-        <v>2.9899999999999984</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>24.14</v>
       </c>
-      <c r="C45">
-        <f t="shared" si="5"/>
-        <v>0.59999999999999787</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>24.74</v>
       </c>
-      <c r="C46">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>23.84</v>
       </c>
-      <c r="C47">
-        <f t="shared" si="5"/>
-        <v>0.89999999999999858</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>22.99</v>
       </c>

</xml_diff>